<commit_message>
M'n verandering misten uit urendocument?
</commit_message>
<xml_diff>
--- a/Urendeclaratie.xlsx
+++ b/Urendeclaratie.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GSS\Documents\GitHub\Empty-Backpack\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -216,7 +221,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -243,9 +248,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="21" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="46" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -515,7 +521,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -526,7 +532,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -594,7 +600,9 @@
       <c r="H3" s="7">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="I3" s="7"/>
+      <c r="I3" s="7">
+        <v>4.1666666666666664E-2</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -619,7 +627,9 @@
       <c r="H4" s="7">
         <v>0.16666666666666666</v>
       </c>
-      <c r="I4" s="7"/>
+      <c r="I4" s="13">
+        <v>0.16666666666666666</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
@@ -644,7 +654,9 @@
       <c r="H5" s="7">
         <v>0</v>
       </c>
-      <c r="I5" s="7"/>
+      <c r="I5" s="7">
+        <v>4.1666666666666664E-2</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
@@ -669,7 +681,9 @@
       <c r="H6" s="7">
         <v>0</v>
       </c>
-      <c r="I6" s="7"/>
+      <c r="I6" s="7">
+        <v>8.3333333333333329E-2</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -692,7 +706,9 @@
       <c r="H7" s="7">
         <v>3.125E-2</v>
       </c>
-      <c r="I7" s="7"/>
+      <c r="I7" s="7">
+        <v>8.3333333333333329E-2</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
@@ -713,7 +729,9 @@
         <v>0</v>
       </c>
       <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
+      <c r="I8" s="7">
+        <v>4.1666666666666664E-2</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
@@ -749,7 +767,7 @@
       </c>
       <c r="I9" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.45833333333333331</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -776,6 +794,9 @@
       <c r="E11" s="7">
         <v>4.1666666666666664E-2</v>
       </c>
+      <c r="I11" s="13">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
@@ -803,6 +824,9 @@
       <c r="E13" s="7">
         <v>4.1666666666666664E-2</v>
       </c>
+      <c r="I13" s="13">
+        <v>1.3888888888888888E-2</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
@@ -813,7 +837,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="I14" s="13">
-        <v>0.16666666666666666</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -840,6 +864,10 @@
       <c r="E16" s="7">
         <f>SUM(E10,E11,E12,E13,E14,E15)</f>
         <v>0.29166666666666663</v>
+      </c>
+      <c r="I16" s="14">
+        <f>SUM(I11,I12,I13,I14,I15)</f>
+        <v>0.4513888888888889</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -888,8 +916,8 @@
         <v>0.23958333333333331</v>
       </c>
       <c r="I18" s="7">
-        <f>SUM(I17,I16,I15,I14,I13,I12,I11)</f>
-        <v>0.35416666666666663</v>
+        <f>SUM(I9,I16)</f>
+        <v>0.90972222222222221</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Uren dennis aangepast, 13,5 -> 1,3 uur
</commit_message>
<xml_diff>
--- a/Urendeclaratie.xlsx
+++ b/Urendeclaratie.xlsx
@@ -531,7 +531,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -542,7 +542,7 @@
   <dimension ref="A1:I60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K63" sqref="K63"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -680,7 +680,7 @@
         <v>3.125E-2</v>
       </c>
       <c r="C6" s="7">
-        <v>0.5625</v>
+        <v>5.5555555555555552E-2</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="7">
@@ -761,7 +761,7 @@
       </c>
       <c r="C9" s="13">
         <f t="shared" ref="C9:I9" si="0">SUM(C3:C8)*24</f>
-        <v>19.5</v>
+        <v>7.3333333333333321</v>
       </c>
       <c r="D9" s="13">
         <f t="shared" si="0"/>
@@ -1564,7 +1564,7 @@
       </c>
       <c r="C60" s="14">
         <f t="shared" ref="C60:I60" si="44">SUM(C58,C51,C44,C37,C30,C23,C16,C9)</f>
-        <v>25.5</v>
+        <v>13.333333333333332</v>
       </c>
       <c r="D60" s="14">
         <f t="shared" si="44"/>

</xml_diff>